<commit_message>
Agent portal steps updated
</commit_message>
<xml_diff>
--- a/src/main/resources/config/demoDevCloud/TestData/TestData.xlsx
+++ b/src/main/resources/config/demoDevCloud/TestData/TestData.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="449">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1368,6 +1368,12 @@
   </si>
   <si>
     <t>TC264321_Embossing File Generation_VISA</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Activated</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1511,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1574,6 +1580,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3383,8 +3393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DN177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
-      <selection activeCell="BZ1" sqref="BZ1"/>
+    <sheetView tabSelected="1" topLeftCell="CU1" workbookViewId="0">
+      <selection activeCell="DD3" sqref="DD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3754,7 +3764,9 @@
       <c r="DM1" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="DN1" s="4"/>
+      <c r="DN1" s="4" t="s">
+        <v>447</v>
+      </c>
     </row>
     <row r="2" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -3993,11 +4005,11 @@
       <c r="CF2" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="CG2" s="9"/>
+      <c r="CG2" s="36"/>
       <c r="CH2" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="CI2" s="28"/>
+      <c r="CI2" s="38"/>
       <c r="CJ2" s="28" t="s">
         <v>133</v>
       </c>
@@ -4060,7 +4072,7 @@
       <c r="DE2" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="DF2" s="9" t="s">
+      <c r="DF2" s="36" t="s">
         <v>425</v>
       </c>
       <c r="DG2" s="9" t="s">
@@ -4083,6 +4095,9 @@
       </c>
       <c r="DM2" s="9" t="s">
         <v>440</v>
+      </c>
+      <c r="DN2" s="39" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="3" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
@@ -4322,11 +4337,11 @@
       <c r="CF3" s="28" t="s">
         <v>402</v>
       </c>
-      <c r="CG3" s="9"/>
+      <c r="CG3" s="36"/>
       <c r="CH3" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="CI3" s="28"/>
+      <c r="CI3" s="38"/>
       <c r="CJ3" s="28" t="s">
         <v>133</v>
       </c>
@@ -4392,26 +4407,29 @@
       <c r="DF3" s="31" t="s">
         <v>425</v>
       </c>
-      <c r="DG3" s="31">
+      <c r="DG3" s="9">
         <v>6</v>
       </c>
-      <c r="DH3" s="31" t="s">
+      <c r="DH3" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="DI3" s="31">
+      <c r="DI3" s="9">
         <v>2</v>
       </c>
-      <c r="DJ3" s="31" t="s">
+      <c r="DJ3" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="DK3" s="31">
+      <c r="DK3" s="9">
         <v>1</v>
       </c>
-      <c r="DL3" s="31" t="s">
+      <c r="DL3" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="DM3" s="31">
+      <c r="DM3" s="9">
         <v>3</v>
+      </c>
+      <c r="DN3" s="39" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
@@ -4649,11 +4667,11 @@
         <v>61</v>
       </c>
       <c r="CF4" s="28"/>
-      <c r="CG4" s="9"/>
+      <c r="CG4" s="36"/>
       <c r="CH4" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="CI4" s="28"/>
+      <c r="CI4" s="38"/>
       <c r="CJ4" s="28" t="s">
         <v>133</v>
       </c>
@@ -4707,13 +4725,16 @@
       <c r="DD4" s="31"/>
       <c r="DE4" s="31"/>
       <c r="DF4" s="31"/>
-      <c r="DG4" s="31"/>
-      <c r="DH4" s="31"/>
-      <c r="DI4" s="31"/>
-      <c r="DJ4" s="31"/>
-      <c r="DK4" s="31"/>
-      <c r="DL4" s="31"/>
-      <c r="DM4" s="31"/>
+      <c r="DG4" s="9"/>
+      <c r="DH4" s="9"/>
+      <c r="DI4" s="9"/>
+      <c r="DJ4" s="9"/>
+      <c r="DK4" s="9"/>
+      <c r="DL4" s="9"/>
+      <c r="DM4" s="9"/>
+      <c r="DN4" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="5" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
@@ -4950,11 +4971,11 @@
         <v>61</v>
       </c>
       <c r="CF5" s="28"/>
-      <c r="CG5" s="9"/>
+      <c r="CG5" s="36"/>
       <c r="CH5" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="CI5" s="28"/>
+      <c r="CI5" s="38"/>
       <c r="CJ5" s="28" t="s">
         <v>133</v>
       </c>
@@ -5008,13 +5029,16 @@
       <c r="DD5" s="31"/>
       <c r="DE5" s="31"/>
       <c r="DF5" s="31"/>
-      <c r="DG5" s="31"/>
-      <c r="DH5" s="31"/>
-      <c r="DI5" s="31"/>
-      <c r="DJ5" s="31"/>
-      <c r="DK5" s="31"/>
-      <c r="DL5" s="31"/>
-      <c r="DM5" s="31"/>
+      <c r="DG5" s="9"/>
+      <c r="DH5" s="9"/>
+      <c r="DI5" s="9"/>
+      <c r="DJ5" s="9"/>
+      <c r="DK5" s="9"/>
+      <c r="DL5" s="9"/>
+      <c r="DM5" s="9"/>
+      <c r="DN5" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="6" spans="1:118" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
@@ -5251,11 +5275,11 @@
         <v>61</v>
       </c>
       <c r="CF6" s="28"/>
-      <c r="CG6" s="9"/>
+      <c r="CG6" s="36"/>
       <c r="CH6" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="CI6" s="28"/>
+      <c r="CI6" s="38"/>
       <c r="CJ6" s="28" t="s">
         <v>133</v>
       </c>
@@ -5309,13 +5333,16 @@
       <c r="DD6" s="31"/>
       <c r="DE6" s="31"/>
       <c r="DF6" s="31"/>
-      <c r="DG6" s="31"/>
-      <c r="DH6" s="31"/>
-      <c r="DI6" s="31"/>
-      <c r="DJ6" s="31"/>
-      <c r="DK6" s="31"/>
-      <c r="DL6" s="31"/>
-      <c r="DM6" s="31"/>
+      <c r="DG6" s="9"/>
+      <c r="DH6" s="9"/>
+      <c r="DI6" s="9"/>
+      <c r="DJ6" s="9"/>
+      <c r="DK6" s="9"/>
+      <c r="DL6" s="9"/>
+      <c r="DM6" s="9"/>
+      <c r="DN6" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="7" spans="1:118" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
@@ -5552,11 +5579,11 @@
         <v>61</v>
       </c>
       <c r="CF7" s="28"/>
-      <c r="CG7" s="9"/>
+      <c r="CG7" s="36"/>
       <c r="CH7" s="28" t="s">
         <v>442</v>
       </c>
-      <c r="CI7" s="28"/>
+      <c r="CI7" s="38"/>
       <c r="CJ7" s="28" t="s">
         <v>133</v>
       </c>
@@ -5610,13 +5637,16 @@
       <c r="DD7" s="31"/>
       <c r="DE7" s="31"/>
       <c r="DF7" s="31"/>
-      <c r="DG7" s="31"/>
-      <c r="DH7" s="31"/>
-      <c r="DI7" s="31"/>
-      <c r="DJ7" s="31"/>
-      <c r="DK7" s="31"/>
-      <c r="DL7" s="31"/>
-      <c r="DM7" s="31"/>
+      <c r="DG7" s="9"/>
+      <c r="DH7" s="9"/>
+      <c r="DI7" s="9"/>
+      <c r="DJ7" s="9"/>
+      <c r="DK7" s="9"/>
+      <c r="DL7" s="9"/>
+      <c r="DM7" s="9"/>
+      <c r="DN7" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="8" spans="1:118" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
@@ -5853,11 +5883,11 @@
         <v>61</v>
       </c>
       <c r="CF8" s="28"/>
-      <c r="CG8" s="9"/>
+      <c r="CG8" s="36"/>
       <c r="CH8" s="28" t="s">
         <v>436</v>
       </c>
-      <c r="CI8" s="28"/>
+      <c r="CI8" s="38"/>
       <c r="CJ8" s="28" t="s">
         <v>133</v>
       </c>
@@ -5911,13 +5941,16 @@
       <c r="DD8" s="31"/>
       <c r="DE8" s="31"/>
       <c r="DF8" s="31"/>
-      <c r="DG8" s="31"/>
-      <c r="DH8" s="31"/>
-      <c r="DI8" s="31"/>
-      <c r="DJ8" s="31"/>
-      <c r="DK8" s="31"/>
-      <c r="DL8" s="31"/>
-      <c r="DM8" s="31"/>
+      <c r="DG8" s="9"/>
+      <c r="DH8" s="9"/>
+      <c r="DI8" s="9"/>
+      <c r="DJ8" s="9"/>
+      <c r="DK8" s="9"/>
+      <c r="DL8" s="9"/>
+      <c r="DM8" s="9"/>
+      <c r="DN8" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="9" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A9" s="31" t="s">
@@ -6155,7 +6188,7 @@
       </c>
       <c r="CF9" s="31"/>
       <c r="CG9" s="31"/>
-      <c r="CH9" s="31">
+      <c r="CH9" s="9">
         <v>552200</v>
       </c>
       <c r="CI9" s="31"/>
@@ -6212,13 +6245,16 @@
       <c r="DD9" s="31"/>
       <c r="DE9" s="31"/>
       <c r="DF9" s="31"/>
-      <c r="DG9" s="31"/>
-      <c r="DH9" s="31"/>
-      <c r="DI9" s="31"/>
-      <c r="DJ9" s="31"/>
-      <c r="DK9" s="31"/>
-      <c r="DL9" s="31"/>
-      <c r="DM9" s="31"/>
+      <c r="DG9" s="9"/>
+      <c r="DH9" s="9"/>
+      <c r="DI9" s="9"/>
+      <c r="DJ9" s="9"/>
+      <c r="DK9" s="9"/>
+      <c r="DL9" s="9"/>
+      <c r="DM9" s="9"/>
+      <c r="DN9" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="10" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A10" s="31" t="s">
@@ -6456,7 +6492,7 @@
       </c>
       <c r="CF10" s="31"/>
       <c r="CG10" s="31"/>
-      <c r="CH10" s="31">
+      <c r="CH10" s="9">
         <v>588765</v>
       </c>
       <c r="CI10" s="31"/>
@@ -6513,13 +6549,16 @@
       <c r="DD10" s="31"/>
       <c r="DE10" s="31"/>
       <c r="DF10" s="31"/>
-      <c r="DG10" s="31"/>
-      <c r="DH10" s="31"/>
-      <c r="DI10" s="31"/>
-      <c r="DJ10" s="31"/>
-      <c r="DK10" s="31"/>
-      <c r="DL10" s="31"/>
-      <c r="DM10" s="31"/>
+      <c r="DG10" s="9"/>
+      <c r="DH10" s="9"/>
+      <c r="DI10" s="9"/>
+      <c r="DJ10" s="9"/>
+      <c r="DK10" s="9"/>
+      <c r="DL10" s="9"/>
+      <c r="DM10" s="9"/>
+      <c r="DN10" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="11" spans="1:118" x14ac:dyDescent="0.3">
       <c r="A11" s="31" t="s">
@@ -6757,7 +6796,7 @@
       </c>
       <c r="CF11" s="31"/>
       <c r="CG11" s="31"/>
-      <c r="CH11" s="31">
+      <c r="CH11" s="9">
         <v>5552200</v>
       </c>
       <c r="CI11" s="31"/>
@@ -6814,16 +6853,29 @@
       <c r="DD11" s="31"/>
       <c r="DE11" s="31"/>
       <c r="DF11" s="31"/>
-      <c r="DG11" s="31"/>
-      <c r="DH11" s="31"/>
-      <c r="DI11" s="31"/>
-      <c r="DJ11" s="31"/>
-      <c r="DK11" s="31"/>
-      <c r="DL11" s="31"/>
-      <c r="DM11" s="31"/>
+      <c r="DG11" s="9"/>
+      <c r="DH11" s="9"/>
+      <c r="DI11" s="9"/>
+      <c r="DJ11" s="9"/>
+      <c r="DK11" s="9"/>
+      <c r="DL11" s="9"/>
+      <c r="DM11" s="9"/>
+      <c r="DN11" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="12" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS12"/>
+      <c r="DG12" s="2"/>
+      <c r="DH12" s="2"/>
+      <c r="DI12" s="2"/>
+      <c r="DJ12" s="2"/>
+      <c r="DK12" s="2"/>
+      <c r="DL12" s="2"/>
+      <c r="DM12" s="2"/>
+      <c r="DN12" s="39" t="s">
+        <v>448</v>
+      </c>
     </row>
     <row r="13" spans="1:118" x14ac:dyDescent="0.3">
       <c r="CS13"/>

</xml_diff>